<commit_message>
order management form testing in progress
</commit_message>
<xml_diff>
--- a/soberano/test_cases/order_test_cases_from_pict_enriched.xlsx
+++ b/soberano/test_cases/order_test_cases_from_pict_enriched.xlsx
@@ -113,6 +113,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -210,11 +211,11 @@
   </sheetPr>
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="262" zoomScaleNormal="262" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:A10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G12" activeCellId="0" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="17.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.8"/>
@@ -222,7 +223,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="16.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="14.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="13.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="13.37"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>